<commit_message>
Customize Menu: Software Version
 - Add Latest Updated Date , Latest Updated By labels
 - Add counter code select box
 - Add Latest Updated Date, Latest Updated By columns in excel
</commit_message>
<xml_diff>
--- a/wwwroot/RegulatorExcel/InputTemplate/SoftwareVersion.xlsx
+++ b/wwwroot/RegulatorExcel/InputTemplate/SoftwareVersion.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">Serial No.</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t xml:space="preserve">FeelView Agent Version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Latest Update User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Latest Update Date</t>
   </si>
 </sst>
 </file>
@@ -237,10 +243,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -249,7 +255,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="43.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="39.86"/>
@@ -288,6 +294,12 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>